<commit_message>
Updated excel sheet with list of bugs
</commit_message>
<xml_diff>
--- a/features/e2e test results.xlsx
+++ b/features/e2e test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalDocker\haal-centraal-proef-omgeving\brpproxy\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043B247E-2240-4488-99DB-5BFD3AB7062A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ABE32B-1286-48AE-9105-32B4868BA022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="0" windowWidth="32430" windowHeight="21000" activeTab="1" xr2:uid="{945C8FCD-65EA-472E-9BB3-ED007FC32D74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="21000" activeTab="2" xr2:uid="{945C8FCD-65EA-472E-9BB3-ED007FC32D74}"/>
   </bookViews>
   <sheets>
     <sheet name="gba-dev" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">algemeen!$B$1:$B$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dev!$B$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'gba-dev'!$B$1:$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dev!$B$1:$B$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'gba-dev'!$B$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="142">
   <si>
     <t>Feature (regel)</t>
   </si>
@@ -54,48 +54,15 @@
     <t>Opmerkingen</t>
   </si>
   <si>
-    <t>features\gba-dev\rni-gba.feature:24</t>
-  </si>
-  <si>
-    <t>features\gba-dev\rni-gba.feature:47</t>
-  </si>
-  <si>
-    <t>features\gba-dev\rni-gba.feature:103</t>
-  </si>
-  <si>
-    <t>features\gba-dev\rni-gba.feature:138</t>
-  </si>
-  <si>
-    <t>features\gba-dev\rni-gba.feature:160</t>
-  </si>
-  <si>
-    <t>features\gba-dev\rni-gba.feature:186</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
-    <t>Melding gemaakt bij GitHub</t>
-  </si>
-  <si>
     <t>GitHub link(s)</t>
   </si>
   <si>
-    <t>https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405 ; https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1406</t>
-  </si>
-  <si>
-    <t>features\gba-dev\kind-geboorte-gba:5</t>
-  </si>
-  <si>
-    <t>features\gba-dev\persoon-geboorte-gba.feature:5</t>
-  </si>
-  <si>
     <t>Logica</t>
   </si>
   <si>
-    <t>https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1376</t>
-  </si>
-  <si>
     <t>features\gba-dev\bag-identificatie.feature:33</t>
   </si>
   <si>
@@ -105,30 +72,6 @@
     <t>features\gba-dev\bag-identificatie.feature:35</t>
   </si>
   <si>
-    <t>Foute verwachting dat er identificaties worden geleverd.</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:221</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:235</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:266</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:267</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:268</t>
-  </si>
-  <si>
-    <t>features\gba-dev\waardetabel-gba.feature:269</t>
-  </si>
-  <si>
-    <t>features\gba-dev\ouders-gba.feature:239</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -144,18 +87,6 @@
     <t>features\dev\kind.feature:86</t>
   </si>
   <si>
-    <t>features\dev\ouder.feature:59</t>
-  </si>
-  <si>
-    <t>features\dev\partner-huwelijk-partnerschap.feature:79</t>
-  </si>
-  <si>
-    <t>features\dev\partner-huwelijk-partnerschap.feature:80</t>
-  </si>
-  <si>
-    <t>features\dev\partner-huwelijk-partnerschap.feature:81</t>
-  </si>
-  <si>
     <t>features\dev\partner-huwelijk-partnerschap.feature:276</t>
   </si>
   <si>
@@ -180,12 +111,6 @@
     <t>features\dev\persoon-adressering-inonderzoek.feature</t>
   </si>
   <si>
-    <t>features\dev\persoon.feature:286</t>
-  </si>
-  <si>
-    <t>features\dev\persoon.feature:287</t>
-  </si>
-  <si>
     <t>features\dev\persoonbeperkt-adressering.feature:5</t>
   </si>
   <si>
@@ -243,9 +168,6 @@
     <t>features\dev\persoonbeperkt-verblijfplaats-locatie.feature:34</t>
   </si>
   <si>
-    <t>features\dev\rni.feature:24</t>
-  </si>
-  <si>
     <t>features\dev\verblijfplaats-binnenland-verblijfadres</t>
   </si>
   <si>
@@ -357,9 +279,6 @@
     <t>features\datum.feature:322</t>
   </si>
   <si>
-    <t>features\datum.feature:404</t>
-  </si>
-  <si>
     <t>features\datum.feature:472</t>
   </si>
   <si>
@@ -393,12 +312,6 @@
     <t>features\gebruik_in_lopende_tekst.feature:474</t>
   </si>
   <si>
-    <t>features\kinderen.feature:144</t>
-  </si>
-  <si>
-    <t>Vermoedelijk proxy.</t>
-  </si>
-  <si>
     <t>features\ouders.feature:249</t>
   </si>
   <si>
@@ -432,45 +345,9 @@
     <t>Vermoedelijk proxy tenzij verborgen logica voor GBA API.</t>
   </si>
   <si>
-    <t>features\kiesrecht.feature:96</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:97</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:98</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:99</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:100</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:153</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:154</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:155</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:156</t>
-  </si>
-  <si>
-    <t>features\kiesrecht.feature:157</t>
-  </si>
-  <si>
-    <t>features\zoek.feature:110</t>
-  </si>
-  <si>
     <t>Proxy</t>
   </si>
   <si>
-    <t>Vraagt met fields maar krijgt een groter object terug dan verwacht. Business logica of fout?</t>
-  </si>
-  <si>
     <t>features\fields.feature</t>
   </si>
   <si>
@@ -480,9 +357,6 @@
     <t>Niet af?</t>
   </si>
   <si>
-    <t>Niet af? (Draait niet. "Parse error in "features\informatievragen-fields.feature" (457:7): inconsistent cell count within the table")</t>
-  </si>
-  <si>
     <t>features\in_onderzoek.feature</t>
   </si>
   <si>
@@ -525,52 +399,91 @@
     <t>Niet af? (Parse error in "features\zoek-met-postcode-huisnummer.feature" (319:5): expected: #EOF, #TableRow, #StepLine, #TagLine, #ExamplesLine, #ScenarioLine, #RuleLine, #Comment, #Empty, got 'n de persoon heeft de volgende 'verblijfplaats' gegevens')</t>
   </si>
   <si>
-    <t>features\waardetabel.feature:261</t>
-  </si>
-  <si>
-    <t>features\waardetabel.feature:275</t>
-  </si>
-  <si>
-    <t>features\waardetabel.feature:307</t>
-  </si>
-  <si>
-    <t>features\waardetabel.feature:308</t>
-  </si>
-  <si>
-    <t>features\waardetabel.feature:309</t>
-  </si>
-  <si>
-    <t>features\waardetabel.feature:310</t>
-  </si>
-  <si>
-    <t>Er wordt een insert gedaan in lo3_adres met een adres_id dat al bestaat en dit gaat verkeerd bij insert en assert.</t>
-  </si>
-  <si>
-    <t>Foutieve verwachting</t>
-  </si>
-  <si>
-    <t>features\gba-dev\partner.feature:96</t>
-  </si>
-  <si>
-    <t>Proxy verwachting bij GBA API</t>
-  </si>
-  <si>
-    <t>features\gba-dev\partner.feature:97</t>
-  </si>
-  <si>
-    <t>features\gba-dev\partner.feature:98</t>
-  </si>
-  <si>
-    <t>https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1429</t>
-  </si>
-  <si>
-    <t>https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1430</t>
-  </si>
-  <si>
     <t>indicatieVestigingVanuitBuitenland wordt alleen bij inOnderzoek getoond. Er wordt ook een daadwerkelijke indicatie verwacht binnen immigratie</t>
   </si>
   <si>
     <t>De verwachting is dat naam als leeg object vanuit de GBA API wordt terug gestuurd. Dit wordt ook gedaan, maar de proxy geeft dit vervolgens ook terug. Is de logica voor het tonen van [] en {} alleen voor de GBA API?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foute verwachting dat er identificaties worden geleverd. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Afhankelijk van resultaat van vraag Cathy bij de RvIG.</t>
+    </r>
+  </si>
+  <si>
+    <t>features\gba-dev\fields-mapping-gba.feature</t>
+  </si>
+  <si>
+    <t>Nog niet omgeschreven.</t>
+  </si>
+  <si>
+    <t>features\dev\partner.feature:173</t>
+  </si>
+  <si>
+    <t>features\dev\partner.feature:190</t>
+  </si>
+  <si>
+    <t>features\dev\partner.feature:207</t>
+  </si>
+  <si>
+    <t>Onderzoeken. Heel de feature gaat ongeveer fout.</t>
+  </si>
+  <si>
+    <t>Onderzoeken. Veel van de feature gaat fout.</t>
+  </si>
+  <si>
+    <t>Niet omgeschreven?</t>
+  </si>
+  <si>
+    <t>Parse error in "features\informatievragen-fields.feature" (457:7): inconsistent cell count within the table
+Parse error in "features\informatievragen-fields.feature" (505:7): inconsistent cell count within the table
+Parse error in "features\informatievragen-fields.feature" (606:7): inconsistent cell count within the table</t>
+  </si>
+  <si>
+    <t>Meer dan 50% gaat fout.</t>
+  </si>
+  <si>
+    <t>features\nationaliteit.feature:18</t>
+  </si>
+  <si>
+    <t>features\nationaliteit.feature:38</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Landelijke tabel sql statement nodig?</t>
+  </si>
+  <si>
+    <t>features\rni.feature:24</t>
+  </si>
+  <si>
+    <t>features\rni.feature:47</t>
+  </si>
+  <si>
+    <t>features\rni.feature:103</t>
+  </si>
+  <si>
+    <t>features\rni.feature:192</t>
+  </si>
+  <si>
+    <t>partner.InOnderzoek maakt onderdeel uit van categorie huwelijk partnerschap. Waarom wordt deze genegeerd omdat de fields een gegeven van deze categorie erbij pakt?</t>
+  </si>
+  <si>
+    <t>features\dev\partner-huwelijk-partnerschap.feature:259</t>
+  </si>
+  <si>
+    <t>Er wordt een bevraging gedaan van een kenmerk van de categorie HuwelijkPartnerschap. Dan hoort InOnderzoek van deze categorie aanwezig te zijn in het response. Zo niet dan spreekt dit logica tegen van In Onderzoek dat eerder is vastgesteld.</t>
   </si>
 </sst>
 </file>
@@ -948,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC51ED-CF2E-4E83-9051-7F70EB9AE199}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,321 +886,66 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>170</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>171</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B7" xr:uid="{5BCC51ED-CF2E-4E83-9051-7F70EB9AE199}"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{FA90CA02-7488-421B-AD2B-FCB53116ABCB}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{414A0FF9-5B0B-499A-A238-6A78D337B87C}"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{1477CA57-FD7A-4BD6-BDCA-D01A4970D45F}"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{B7E7C10B-50C8-4D5C-B22D-E2AE5074594F}"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{946771F5-A285-4349-9583-53FD6AF2F171}"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1405" xr:uid="{19815D47-1574-4E14-A7E2-1F8D68B94FF0}"/>
-    <hyperlink ref="D9:D15" r:id="rId7" display="https://github.com/VNG-Realisatie/Haal-Centraal-BRP-bevragen/issues/1376" xr:uid="{C9D8CE57-9A69-4E5B-B52E-94404BD99709}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{9ED5B4F6-C694-488C-AA6B-45327BE9EE6D}"/>
-    <hyperlink ref="D19" r:id="rId9" xr:uid="{7C1110F4-4507-40E9-BF8E-29935335A5AB}"/>
-    <hyperlink ref="D20" r:id="rId10" xr:uid="{53B4B3F8-CBC6-4302-9792-DCFA881B5A55}"/>
-    <hyperlink ref="D21" r:id="rId11" xr:uid="{502AD170-A644-4CCE-8373-0890B1D1706C}"/>
-    <hyperlink ref="D22" r:id="rId12" xr:uid="{21E0AE6C-780A-469D-AFA1-F78CBA276058}"/>
-  </hyperlinks>
+  <autoFilter ref="B1" xr:uid="{5BCC51ED-CF2E-4E83-9051-7F70EB9AE199}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8FCB5A-B662-42C7-A82C-D200097F581F}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,579 +967,543 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B9" xr:uid="{9A8FCB5A-B662-42C7-A82C-D200097F581F}"/>
+  <autoFilter ref="B1:B5" xr:uid="{9A8FCB5A-B662-42C7-A82C-D200097F581F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30C5A75-9C27-4210-8CF6-7479724AF019}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,801 +1525,623 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>135</v>
       </c>
-      <c r="B54" t="s">
-        <v>140</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
-        <v>140</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>137</v>
       </c>
-      <c r="B56" t="s">
-        <v>140</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>138</v>
       </c>
-      <c r="B57" t="s">
-        <v>140</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>139</v>
-      </c>
       <c r="B58" t="s">
-        <v>140</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>152</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>153</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>154</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>155</v>
-      </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>156</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>157</v>
-      </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>158</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>161</v>
-      </c>
-      <c r="B75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>162</v>
-      </c>
-      <c r="B76" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>163</v>
-      </c>
-      <c r="B77" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>164</v>
-      </c>
-      <c r="B78" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:B15" xr:uid="{C30C5A75-9C27-4210-8CF6-7479724AF019}"/>
-  <hyperlinks>
-    <hyperlink ref="D74" r:id="rId1" xr:uid="{9B91F55A-88AE-4630-8167-7BFC468E1F06}"/>
-    <hyperlink ref="D75" r:id="rId2" xr:uid="{79AE226A-207D-4EAF-B9C7-182A1EEC1174}"/>
-    <hyperlink ref="D76" r:id="rId3" xr:uid="{9CDC0D77-460E-4D2C-A488-EEB49C3C21B6}"/>
-    <hyperlink ref="D77" r:id="rId4" xr:uid="{E1545BC4-5A72-4E8A-A71E-BAE6379480DC}"/>
-    <hyperlink ref="D78" r:id="rId5" xr:uid="{9B653A02-908D-4443-957B-F63B66558C45}"/>
-    <hyperlink ref="D79" r:id="rId6" xr:uid="{D0452224-1C71-471C-8189-2576E0CE01EB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fails doorgenomen. Nog niet af
</commit_message>
<xml_diff>
--- a/features/e2e test results.xlsx
+++ b/features/e2e test results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalDocker\haal-centraal-proef-omgeving\brpproxy\features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\GitHub\Haal-Centraal-BRP-bevragen\features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ABE32B-1286-48AE-9105-32B4868BA022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E137625-366F-4B5C-A3A7-00E18CE7CC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="21000" activeTab="2" xr2:uid="{945C8FCD-65EA-472E-9BB3-ED007FC32D74}"/>
+    <workbookView xWindow="49980" yWindow="240" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{945C8FCD-65EA-472E-9BB3-ED007FC32D74}"/>
   </bookViews>
   <sheets>
     <sheet name="gba-dev" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
   <si>
     <t>Feature (regel)</t>
   </si>
@@ -484,6 +484,33 @@
   </si>
   <si>
     <t>Er wordt een bevraging gedaan van een kenmerk van de categorie HuwelijkPartnerschap. Dan hoort InOnderzoek van deze categorie aanwezig te zijn in het response. Zo niet dan spreekt dit logica tegen van In Onderzoek dat eerder is vastgesteld.</t>
+  </si>
+  <si>
+    <t>Geen Gba fout. Aanroep naar GBA-API werkt.  (Conform gba-field-mappings )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geen Gba fout. Aanroep naar GBA-API werkt.  (Conform gba-field-mappings ) Wel de vraag of bij gba-fields-mapping ook niet openbarerRuimteNaam en/of gemeentcode moeten worden opgenomen.  </t>
+  </si>
+  <si>
+    <t>Geen Gba fout. Aanroep naar GBA-API werkt.  (Conform afspraken in Onderzoek )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hier levert de GBA-API een lege verblijfplaats. Er zou echter een veblijfplaats met een datumAanvangAdreshouding geleverd moeten worden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hier levert de GBA-API een verblijfplaats met een datumAanvangAdreshouding. Dit zou een datumAanvangAdresBuitenland moeten zijn.  </t>
+  </si>
+  <si>
+    <t>features\gebruik_in_lopende_tekst.feature:471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deze is nog in behandeling bij Robert. </t>
+  </si>
+  <si>
+    <t>Ook nog in behandeling bij Robert</t>
+  </si>
+  <si>
+    <t>3 fouten (gboorte wordt foutief ge-insert) Veel scenarios zijn niet verifieerbaar</t>
   </si>
 </sst>
 </file>
@@ -536,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -546,10 +573,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,7 +607,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1500,643 +1542,766 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30C5A75-9C27-4210-8CF6-7479724AF019}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="139.42578125" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="139.42578125" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="225" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="8" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="D39" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="D40" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D41" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="B47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="4" t="s">
+      <c r="B48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="B49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="B50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="4" t="s">
+      <c r="B51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="4" t="s">
+      <c r="B52" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="4" t="s">
+      <c r="B53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="4" t="s">
+      <c r="B54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C55" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B56" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B58" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C60" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C61" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C65" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="8" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>